<commit_message>
fixed the example file. removed the headers.
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/examples/NewLineFormat.xlsx
+++ b/src/main/webapp/resources/examples/NewLineFormat.xlsx
@@ -22,22 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t xml:space="preserve">Company name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Site</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telephone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comment</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Company 1</t>
   </si>
@@ -131,18 +116,12 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -182,7 +161,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -191,6 +170,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -199,7 +182,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -221,97 +208,84 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9230769230769"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="29.9919028340081"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3400809716599"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5991902834008"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="F3" s="6"/>
     </row>
-    <row r="4" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="user1@mail.com"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://site-2.com"/>
-    <hyperlink ref="C3" r:id="rId3" display="user2@mail.com"/>
-    <hyperlink ref="B4" r:id="rId4" display="http://site-3.com"/>
-    <hyperlink ref="C4" r:id="rId5" display="user3@mail.com"/>
+    <hyperlink ref="C1" r:id="rId1" display="user1@mail.com"/>
+    <hyperlink ref="B2" r:id="rId2" display="http://site-2.com"/>
+    <hyperlink ref="C2" r:id="rId3" display="user2@mail.com"/>
+    <hyperlink ref="B3" r:id="rId4" display="http://site-3.com"/>
+    <hyperlink ref="C3" r:id="rId5" display="user3@mail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Column category #7 Added column category did some localization and cleaning thus changed the example files
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/examples/NewLineFormat.xlsx
+++ b/src/main/webapp/resources/examples/NewLineFormat.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Company 1</t>
   </si>
@@ -36,7 +36,10 @@
     <t xml:space="preserve">+1 448 542 8235</t>
   </si>
   <si>
-    <t xml:space="preserve">speedflowda</t>
+    <t xml:space="preserve">Comment ko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 1</t>
   </si>
   <si>
     <t xml:space="preserve">Company 2</t>
@@ -51,7 +54,10 @@
     <t xml:space="preserve">+52 55 8503 5058</t>
   </si>
   <si>
-    <t xml:space="preserve">speedflowbest</t>
+    <t xml:space="preserve">Comment koko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 2</t>
   </si>
   <si>
     <t xml:space="preserve">Company 3</t>
@@ -66,7 +72,10 @@
     <t xml:space="preserve"> +48 22 51 56 100</t>
   </si>
   <si>
-    <t xml:space="preserve">speedflowever</t>
+    <t xml:space="preserve">Comment kokoko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category 3</t>
   </si>
 </sst>
 </file>
@@ -161,7 +170,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -183,10 +192,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -210,18 +215,19 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5991902834008"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -240,43 +246,49 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6"/>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="6"/>
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>